<commit_message>
Updated compatibility_blacklist excel file to empty
</commit_message>
<xml_diff>
--- a/data/compatibility_blacklist.xlsx
+++ b/data/compatibility_blacklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tigo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bathcraft-my.sharepoint.com/personal/olep00903843_maax_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A84474DF-A7F9-423D-8B5A-50154E6677B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{206B7547-17BE-4FFB-8347-6BD8EE67B904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E9D806C-D0A3-44D9-BE90-865369E10F0A}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="2070" windowWidth="21600" windowHeight="11423" xr2:uid="{B4D32BDF-BA2C-4A1D-88F6-FD125EA98F8A}"/>
+    <workbookView xWindow="28680" yWindow="-2730" windowWidth="38640" windowHeight="21120" xr2:uid="{8EDA3920-48F0-4724-A969-C48E638174CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>SKU 1</t>
+    <t xml:space="preserve">SKU 1 </t>
   </si>
   <si>
     <t>SKU 2</t>
@@ -77,11 +77,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,32 +412,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B0A842-D8F8-4D31-8754-B2AD3A99972B}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF02477C-32F7-4DE6-8DE1-53F2FC666413}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="2" width="9.06640625" style="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="1">
-        <v>105821</v>
-      </c>
-      <c r="B2" s="1">
-        <v>139398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>